<commit_message>
Finished RNAi access and put all column and table names in a config files
</commit_message>
<xml_diff>
--- a/src/test_data/RNAi_lookup_test_data.xlsx
+++ b/src/test_data/RNAi_lookup_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattias/Documents/coding/gene_data_explorer/src/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E126CF8-BC8D-C340-AD7B-AC147429816F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D51FA1-2591-7D47-A7FB-CDF596626767}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21160" yWindow="4620" windowWidth="27640" windowHeight="16940" xr2:uid="{59EECF98-CB5B-B54F-B9ED-4C02391B1513}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>WBGene00012198</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>ahringer well</t>
-  </si>
-  <si>
-    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -508,7 +505,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,12 +641,6 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -681,18 +672,6 @@
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
       <c r="G8" t="s">
         <v>24</v>
       </c>
@@ -726,15 +705,6 @@
       </c>
       <c r="B10" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
       </c>
       <c r="F10">
         <v>81</v>

</xml_diff>